<commit_message>
all files up to date
</commit_message>
<xml_diff>
--- a/ConsolidadedResultsPhantomExpanded.xlsx
+++ b/ConsolidadedResultsPhantomExpanded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardobertini/RProjects/CoralMethodsPaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA283C8-9FD1-0A47-9FAD-D27B98AE5DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81083C00-75EE-BC46-B26C-00E37D661E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,26 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={BBF0D43F-D855-7248-8974-09E8877BBEB9}</author>
-  </authors>
-  <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{BBF0D43F-D855-7248-8974-09E8877BBEB9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Should have 6 points. Remove Air and run again</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="317">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -391,30 +373,6 @@
     <t>LB_0031_PNormal</t>
   </si>
   <si>
-    <t>Poly3_AllPoints_n7</t>
-  </si>
-  <si>
-    <t>[0.001225, 1.13, 1.26, 1.44, 1.65, 1.77, 1.92]</t>
-  </si>
-  <si>
-    <t>[19611.58, 30083.36, 31711.8, 34008.78, 36201.44, 37724.74, 39447.42]</t>
-  </si>
-  <si>
-    <t>['air', 'epoxy', 'insert1', 'insert2', 'insert3', 'insert4', 'insert5']</t>
-  </si>
-  <si>
-    <t>['(255, 255, 255)', '(0, 0, 255)', '(0, 255, 0)', '(255, 0, 0)', '(0, 255, 255)', '(255, 255, 0)', '(255, 0, 255)']</t>
-  </si>
-  <si>
-    <t>[-1212.2751660749866, 4943.880491735611, 5290.450637389322, 19603.53151251024]</t>
-  </si>
-  <si>
-    <t>[19610.01973122322, 30145.39353235327, 31693.397836687822, 33853.57676851657, 36346.79812254822, 37733.96407724834, 39405.969930371735]</t>
-  </si>
-  <si>
-    <t>[1.5602687767823227, -62.03353235327086, 18.402163312177436, 155.20323148342868, -145.3581225482194, -9.224077248341928, 41.45006962826301]</t>
-  </si>
-  <si>
     <t>[19611.58, 20703.42, 22388.77, 28316.82, 30083.36, 31711.8, 34008.78, 36201.44, 37724.74, 39447.42, 45096.31]</t>
   </si>
   <si>
@@ -1001,13 +959,25 @@
   </si>
   <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>[30107.03, 31745.03, 34008.51, 36231.89, 37648.13, 39306.02]</t>
+  </si>
+  <si>
+    <t>[3072.5457262814907, -15387.45583625941, 36684.73329940086, 3852.477556639823]</t>
+  </si>
+  <si>
+    <t>[30091.35083845754, 31792.363357995528, 33945.637463654464, 36292.19845710724, 37615.07706254733, 39309.982822201826]</t>
+  </si>
+  <si>
+    <t>[15.679161542459042, -47.333357995528786, 62.87253634553781, -60.30845710723952, 33.05293745266681, -3.9628222018291126]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,20 +989,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1071,12 +1027,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,9 +1050,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Leonardo Bertini" id="{A1EBBE25-4DC4-D641-BD94-FD1851D0F267}" userId="d37d80f881b5f91f" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1383,20 +1336,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D18" dT="2023-01-18T18:54:34.34" personId="{A1EBBE25-4DC4-D641-BD94-FD1851D0F267}" id="{BBF0D43F-D855-7248-8974-09E8877BBEB9}">
-    <text>Should have 6 points. Remove Air and run again</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:G61"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1424,10 +1369,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1516,10 +1461,10 @@
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -1608,10 +1553,10 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
@@ -1700,10 +1645,10 @@
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G4" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -1792,10 +1737,10 @@
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G5" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -1884,10 +1829,10 @@
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G6" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
@@ -1976,10 +1921,10 @@
         <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G7" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -2068,10 +2013,10 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G8" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
@@ -2160,10 +2105,10 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G9" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H9" t="s">
         <v>29</v>
@@ -2252,10 +2197,10 @@
         <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G10" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H10" t="s">
         <v>38</v>
@@ -2344,10 +2289,10 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G11" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -2436,10 +2381,10 @@
         <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G12" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -2528,10 +2473,10 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G13" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
@@ -2620,10 +2565,10 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G14" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -2712,10 +2657,10 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G15" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -2804,10 +2749,10 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G16" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>
@@ -2896,10 +2841,10 @@
         <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G17" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>
@@ -2981,59 +2926,59 @@
       <c r="C18" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>117</v>
+      <c r="E18" t="s">
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G18" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H18" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>313</v>
       </c>
       <c r="J18" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="L18" t="s">
-        <v>122</v>
+        <v>314</v>
       </c>
       <c r="M18">
-        <v>0.99980593438771725</v>
+        <v>0.99982087381395046</v>
       </c>
       <c r="N18" t="s">
-        <v>123</v>
+        <v>315</v>
       </c>
       <c r="O18" t="s">
-        <v>124</v>
+        <v>316</v>
       </c>
       <c r="P18">
-        <v>51209.4519163613</v>
+        <v>11184.549345037351</v>
       </c>
       <c r="Q18">
-        <v>226.29505499758781</v>
+        <v>105.7570297665236</v>
       </c>
       <c r="R18">
-        <v>1061.6728628374351</v>
+        <v>1093.1230321705709</v>
       </c>
       <c r="S18">
         <v>868.76254528963523</v>
       </c>
       <c r="T18">
-        <v>-1.6414027517917519E-2</v>
+        <v>1.2722956642706359E-2</v>
       </c>
       <c r="U18">
-        <v>1.222051835215209</v>
+        <v>1.25825294621344</v>
       </c>
       <c r="V18">
         <v>63.01707445872205</v>
@@ -3080,16 +3025,16 @@
         <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G19" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H19" t="s">
         <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J19" t="s">
         <v>31</v>
@@ -3098,16 +3043,16 @@
         <v>32</v>
       </c>
       <c r="L19" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="M19">
         <v>0.99858670800352134</v>
       </c>
       <c r="N19" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="O19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="P19">
         <v>944267.66235134925</v>
@@ -3163,25 +3108,25 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
         <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G20" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
       </c>
       <c r="I20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J20" t="s">
         <v>40</v>
@@ -3190,16 +3135,16 @@
         <v>41</v>
       </c>
       <c r="L20" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="M20">
         <v>0.99997313889481587</v>
       </c>
       <c r="N20" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="P20">
         <v>2081.7990214385259</v>
@@ -3255,25 +3200,25 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G21" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J21" t="s">
         <v>31</v>
@@ -3282,16 +3227,16 @@
         <v>32</v>
       </c>
       <c r="L21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="M21">
         <v>0.99744462587606453</v>
       </c>
       <c r="N21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="P21">
         <v>1664467.4917226869</v>
@@ -3347,25 +3292,25 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G22" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H22" t="s">
         <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J22" t="s">
         <v>40</v>
@@ -3374,16 +3319,16 @@
         <v>41</v>
       </c>
       <c r="L22" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="M22">
         <v>0.99994112495737852</v>
       </c>
       <c r="N22" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="O22" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="P22">
         <v>4757.9033966089992</v>
@@ -3439,25 +3384,25 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G23" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H23" t="s">
         <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J23" t="s">
         <v>31</v>
@@ -3466,16 +3411,16 @@
         <v>32</v>
       </c>
       <c r="L23" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="M23">
         <v>0.99735237412817157</v>
       </c>
       <c r="N23" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="O23" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="P23">
         <v>1802638.153948318</v>
@@ -3531,25 +3476,25 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F24" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G24" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="J24" t="s">
         <v>40</v>
@@ -3558,16 +3503,16 @@
         <v>41</v>
       </c>
       <c r="L24" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="M24">
         <v>0.99978564298501227</v>
       </c>
       <c r="N24" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="O24" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="P24">
         <v>13330.27210184553</v>
@@ -3623,25 +3568,25 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G25" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="J25" t="s">
         <v>31</v>
@@ -3650,16 +3595,16 @@
         <v>32</v>
       </c>
       <c r="L25" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="M25">
         <v>0.99882147922086639</v>
       </c>
       <c r="N25" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="O25" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="P25">
         <v>752257.45083807933</v>
@@ -3715,25 +3660,25 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G26" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H26" t="s">
         <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="J26" t="s">
         <v>31</v>
@@ -3742,16 +3687,16 @@
         <v>32</v>
       </c>
       <c r="L26" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="M26">
         <v>0.99858721933786732</v>
       </c>
       <c r="N26" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="O26" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P26">
         <v>957956.92669416789</v>
@@ -3807,25 +3752,25 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E27" t="s">
         <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G27" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H27" t="s">
         <v>38</v>
       </c>
       <c r="I27" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="J27" t="s">
         <v>40</v>
@@ -3834,16 +3779,16 @@
         <v>41</v>
       </c>
       <c r="L27" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="M27">
         <v>0.99999673893262497</v>
       </c>
       <c r="N27" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O27" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="P27">
         <v>215.2741670487685</v>
@@ -3899,25 +3844,25 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E28" t="s">
         <v>37</v>
       </c>
       <c r="F28" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G28" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H28" t="s">
         <v>38</v>
       </c>
       <c r="I28" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="J28" t="s">
         <v>40</v>
@@ -3926,16 +3871,16 @@
         <v>41</v>
       </c>
       <c r="L28" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="M28">
         <v>0.9999313708469717</v>
       </c>
       <c r="N28" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="O28" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="P28">
         <v>4599.7948357433806</v>
@@ -3991,25 +3936,25 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E29" t="s">
         <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G29" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H29" t="s">
         <v>29</v>
       </c>
       <c r="I29" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J29" t="s">
         <v>31</v>
@@ -4018,16 +3963,16 @@
         <v>32</v>
       </c>
       <c r="L29" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="M29">
         <v>0.99876724264055317</v>
       </c>
       <c r="N29" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="O29" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="P29">
         <v>857947.87397254014</v>
@@ -4083,25 +4028,25 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E30" t="s">
         <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G30" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H30" t="s">
         <v>38</v>
       </c>
       <c r="I30" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="J30" t="s">
         <v>40</v>
@@ -4110,16 +4055,16 @@
         <v>41</v>
       </c>
       <c r="L30" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="M30">
         <v>0.99981590202266701</v>
       </c>
       <c r="N30" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="O30" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="P30">
         <v>12445.85455291554</v>
@@ -4175,25 +4120,25 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E31" t="s">
         <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G31" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H31" t="s">
         <v>29</v>
       </c>
       <c r="I31" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="J31" t="s">
         <v>31</v>
@@ -4202,16 +4147,16 @@
         <v>32</v>
       </c>
       <c r="L31" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="M31">
         <v>0.99879082976865985</v>
       </c>
       <c r="N31" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="O31" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="P31">
         <v>847370.34817103099</v>
@@ -4267,25 +4212,25 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D32" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G32" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H32" t="s">
         <v>38</v>
       </c>
       <c r="I32" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="J32" t="s">
         <v>40</v>
@@ -4294,16 +4239,16 @@
         <v>41</v>
       </c>
       <c r="L32" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="M32">
         <v>0.99990609393501906</v>
       </c>
       <c r="N32" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="O32" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="P32">
         <v>6180.0860017213199</v>
@@ -4359,25 +4304,25 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D33" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E33" t="s">
         <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G33" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H33" t="s">
         <v>29</v>
       </c>
       <c r="I33" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="J33" t="s">
         <v>31</v>
@@ -4386,16 +4331,16 @@
         <v>32</v>
       </c>
       <c r="L33" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M33">
         <v>0.99893185694917908</v>
       </c>
       <c r="N33" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="O33" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="P33">
         <v>739716.54942673049</v>
@@ -4451,25 +4396,25 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D34" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E34" t="s">
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G34" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H34" t="s">
         <v>29</v>
       </c>
       <c r="I34" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="J34" t="s">
         <v>31</v>
@@ -4478,16 +4423,16 @@
         <v>32</v>
       </c>
       <c r="L34" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="M34">
         <v>0.99895323621912568</v>
       </c>
       <c r="N34" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="O34" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="P34">
         <v>1016135.856803235</v>
@@ -4543,25 +4488,25 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
       <c r="F35" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G35" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H35" t="s">
         <v>38</v>
       </c>
       <c r="I35" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J35" t="s">
         <v>40</v>
@@ -4570,16 +4515,16 @@
         <v>41</v>
       </c>
       <c r="L35" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="M35">
         <v>0.99994523371582622</v>
       </c>
       <c r="N35" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="O35" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P35">
         <v>5006.6520254361876</v>
@@ -4635,25 +4580,25 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D36" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E36" t="s">
         <v>28</v>
       </c>
       <c r="F36" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G36" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H36" t="s">
         <v>29</v>
       </c>
       <c r="I36" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="J36" t="s">
         <v>31</v>
@@ -4662,16 +4607,16 @@
         <v>32</v>
       </c>
       <c r="L36" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="M36">
         <v>0.99874552618261225</v>
       </c>
       <c r="N36" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="O36" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="P36">
         <v>861140.65285099135</v>
@@ -4727,25 +4672,25 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E37" t="s">
         <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G37" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H37" t="s">
         <v>38</v>
       </c>
       <c r="I37" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="J37" t="s">
         <v>40</v>
@@ -4754,16 +4699,16 @@
         <v>41</v>
       </c>
       <c r="L37" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="M37">
         <v>0.99991475910755045</v>
       </c>
       <c r="N37" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="O37" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="P37">
         <v>5659.5896804126278</v>
@@ -4819,25 +4764,25 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D38" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E38" t="s">
         <v>28</v>
       </c>
       <c r="F38" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G38" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H38" t="s">
         <v>29</v>
       </c>
       <c r="I38" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="J38" t="s">
         <v>31</v>
@@ -4846,16 +4791,16 @@
         <v>32</v>
       </c>
       <c r="L38" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="M38">
         <v>0.99864875687614507</v>
       </c>
       <c r="N38" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="O38" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="P38">
         <v>943261.00294229807</v>
@@ -4911,25 +4856,25 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D39" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E39" t="s">
         <v>37</v>
       </c>
       <c r="F39" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G39" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H39" t="s">
         <v>38</v>
       </c>
       <c r="I39" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J39" t="s">
         <v>40</v>
@@ -4938,16 +4883,16 @@
         <v>41</v>
       </c>
       <c r="L39" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="M39">
         <v>0.9999829321418845</v>
       </c>
       <c r="N39" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="O39" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="P39">
         <v>1154.0112704476039</v>
@@ -5003,25 +4948,25 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D40" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
       </c>
       <c r="F40" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G40" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H40" t="s">
         <v>38</v>
       </c>
       <c r="I40" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J40" t="s">
         <v>40</v>
@@ -5030,16 +4975,16 @@
         <v>41</v>
       </c>
       <c r="L40" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="M40">
         <v>0.99988186321641559</v>
       </c>
       <c r="N40" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="O40" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="P40">
         <v>7982.3309638047231</v>
@@ -5095,25 +5040,25 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D41" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E41" t="s">
         <v>28</v>
       </c>
       <c r="F41" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G41" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H41" t="s">
         <v>29</v>
       </c>
       <c r="I41" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J41" t="s">
         <v>31</v>
@@ -5122,16 +5067,16 @@
         <v>32</v>
       </c>
       <c r="L41" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M41">
         <v>0.99864487481543796</v>
       </c>
       <c r="N41" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="O41" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="P41">
         <v>947809.25684309739</v>
@@ -5187,25 +5132,25 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D42" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E42" t="s">
         <v>28</v>
       </c>
       <c r="F42" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G42" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H42" t="s">
         <v>29</v>
       </c>
       <c r="I42" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J42" t="s">
         <v>31</v>
@@ -5214,16 +5159,16 @@
         <v>32</v>
       </c>
       <c r="L42" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M42">
         <v>0.99864487481543796</v>
       </c>
       <c r="N42" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="O42" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="P42">
         <v>947809.25684309739</v>
@@ -5279,25 +5224,25 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D43" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E43" t="s">
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G43" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H43" t="s">
         <v>38</v>
       </c>
       <c r="I43" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J43" t="s">
         <v>40</v>
@@ -5306,16 +5251,16 @@
         <v>41</v>
       </c>
       <c r="L43" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="M43">
         <v>0.99988186321641559</v>
       </c>
       <c r="N43" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="O43" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="P43">
         <v>7982.3309638047231</v>
@@ -5371,25 +5316,25 @@
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D44" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E44" t="s">
         <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G44" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H44" t="s">
         <v>29</v>
       </c>
       <c r="I44" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J44" t="s">
         <v>31</v>
@@ -5398,16 +5343,16 @@
         <v>32</v>
       </c>
       <c r="L44" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M44">
         <v>0.99864487481543796</v>
       </c>
       <c r="N44" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="O44" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="P44">
         <v>947809.25684309739</v>
@@ -5463,25 +5408,25 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D45" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E45" t="s">
         <v>37</v>
       </c>
       <c r="F45" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G45" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H45" t="s">
         <v>38</v>
       </c>
       <c r="I45" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J45" t="s">
         <v>40</v>
@@ -5490,16 +5435,16 @@
         <v>41</v>
       </c>
       <c r="L45" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="M45">
         <v>0.99988186321641559</v>
       </c>
       <c r="N45" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="O45" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="P45">
         <v>7982.3309638047231</v>
@@ -5555,25 +5500,25 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
       <c r="F46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G46" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H46" t="s">
         <v>29</v>
       </c>
       <c r="I46" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="J46" t="s">
         <v>31</v>
@@ -5582,16 +5527,16 @@
         <v>32</v>
       </c>
       <c r="L46" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="M46">
         <v>0.9986594499795497</v>
       </c>
       <c r="N46" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="O46" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="P46">
         <v>947904.35424197593</v>
@@ -5647,25 +5592,25 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D47" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E47" t="s">
         <v>37</v>
       </c>
       <c r="F47" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G47" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H47" t="s">
         <v>38</v>
       </c>
       <c r="I47" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J47" t="s">
         <v>40</v>
@@ -5674,16 +5619,16 @@
         <v>41</v>
       </c>
       <c r="L47" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="M47">
         <v>0.99988583361336947</v>
       </c>
       <c r="N47" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="O47" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="P47">
         <v>7830.6313005124712</v>
@@ -5739,25 +5684,25 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D48" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E48" t="s">
         <v>28</v>
       </c>
       <c r="F48" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G48" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H48" t="s">
         <v>29</v>
       </c>
       <c r="I48" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="J48" t="s">
         <v>31</v>
@@ -5766,16 +5711,16 @@
         <v>32</v>
       </c>
       <c r="L48" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="M48">
         <v>0.99881403943162961</v>
       </c>
       <c r="N48" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="O48" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="P48">
         <v>817310.33120256383</v>
@@ -5831,25 +5776,25 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D49" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E49" t="s">
         <v>37</v>
       </c>
       <c r="F49" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G49" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H49" t="s">
         <v>38</v>
       </c>
       <c r="I49" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="J49" t="s">
         <v>40</v>
@@ -5858,16 +5803,16 @@
         <v>41</v>
       </c>
       <c r="L49" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="M49">
         <v>0.99987077943686908</v>
       </c>
       <c r="N49" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O49" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="P49">
         <v>8625.4984090901653</v>
@@ -5923,25 +5868,25 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D50" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E50" t="s">
         <v>28</v>
       </c>
       <c r="F50" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G50" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H50" t="s">
         <v>29</v>
       </c>
       <c r="I50" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="J50" t="s">
         <v>31</v>
@@ -5950,16 +5895,16 @@
         <v>32</v>
       </c>
       <c r="L50" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="M50">
         <v>0.99864498686790382</v>
       </c>
       <c r="N50" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="O50" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="P50">
         <v>961609.37350798131</v>
@@ -6015,25 +5960,25 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D51" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E51" t="s">
         <v>37</v>
       </c>
       <c r="F51" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G51" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>
       </c>
       <c r="I51" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="J51" t="s">
         <v>40</v>
@@ -6042,16 +5987,16 @@
         <v>41</v>
       </c>
       <c r="L51" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="M51">
         <v>0.99995635091134072</v>
       </c>
       <c r="N51" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="O51" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="P51">
         <v>3062.5489598835611</v>
@@ -6107,25 +6052,25 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D52" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="E52" t="s">
         <v>28</v>
       </c>
       <c r="F52" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G52" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H52" t="s">
         <v>29</v>
       </c>
       <c r="I52" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="J52" t="s">
         <v>31</v>
@@ -6134,16 +6079,16 @@
         <v>32</v>
       </c>
       <c r="L52" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="M52">
         <v>0.99892534691161416</v>
       </c>
       <c r="N52" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="O52" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="P52">
         <v>687972.91847450985</v>
@@ -6199,25 +6144,25 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D53" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="E53" t="s">
         <v>37</v>
       </c>
       <c r="F53" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G53" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H53" t="s">
         <v>38</v>
       </c>
       <c r="I53" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="J53" t="s">
         <v>40</v>
@@ -6226,16 +6171,16 @@
         <v>41</v>
       </c>
       <c r="L53" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="M53">
         <v>0.999536724346476</v>
       </c>
       <c r="N53" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="O53" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="P53">
         <v>27792.34437001247</v>
@@ -6291,25 +6236,25 @@
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D54" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E54" t="s">
         <v>37</v>
       </c>
       <c r="F54" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G54" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H54" t="s">
         <v>38</v>
       </c>
       <c r="I54" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="J54" t="s">
         <v>40</v>
@@ -6318,16 +6263,16 @@
         <v>41</v>
       </c>
       <c r="L54" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="M54">
         <v>0.99992899317154882</v>
       </c>
       <c r="N54" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="O54" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="P54">
         <v>4129.9125892495358</v>
@@ -6383,25 +6328,25 @@
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D55" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E55" t="s">
         <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G55" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H55" t="s">
         <v>29</v>
       </c>
       <c r="I55" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="J55" t="s">
         <v>31</v>
@@ -6410,16 +6355,16 @@
         <v>32</v>
       </c>
       <c r="L55" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="M55">
         <v>0.99898940147146886</v>
       </c>
       <c r="N55" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="O55" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="P55">
         <v>626436.26479329634</v>
@@ -6475,25 +6420,25 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D56" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E56" t="s">
         <v>28</v>
       </c>
       <c r="F56" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G56" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H56" t="s">
         <v>29</v>
       </c>
       <c r="I56" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="J56" t="s">
         <v>31</v>
@@ -6502,16 +6447,16 @@
         <v>32</v>
       </c>
       <c r="L56" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="M56">
         <v>0.99898940147146886</v>
       </c>
       <c r="N56" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="O56" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="P56">
         <v>626436.26479329634</v>
@@ -6567,25 +6512,25 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D57" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E57" t="s">
         <v>37</v>
       </c>
       <c r="F57" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G57" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H57" t="s">
         <v>38</v>
       </c>
       <c r="I57" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="J57" t="s">
         <v>40</v>
@@ -6594,16 +6539,16 @@
         <v>41</v>
       </c>
       <c r="L57" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="M57">
         <v>0.99992899317154882</v>
       </c>
       <c r="N57" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="O57" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="P57">
         <v>4129.9125892495358</v>
@@ -6659,25 +6604,25 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D58" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E58" t="s">
         <v>37</v>
       </c>
       <c r="F58" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G58" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H58" t="s">
         <v>38</v>
       </c>
       <c r="I58" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J58" t="s">
         <v>40</v>
@@ -6686,16 +6631,16 @@
         <v>41</v>
       </c>
       <c r="L58" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="M58">
         <v>0.99982859105768773</v>
       </c>
       <c r="N58" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="O58" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="P58">
         <v>15216.174037177399</v>
@@ -6751,25 +6696,25 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E59" t="s">
         <v>28</v>
       </c>
       <c r="F59" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G59" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H59" t="s">
         <v>29</v>
       </c>
       <c r="I59" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="J59" t="s">
         <v>31</v>
@@ -6778,16 +6723,16 @@
         <v>32</v>
       </c>
       <c r="L59" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="M59">
         <v>0.99901002099263114</v>
       </c>
       <c r="N59" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="O59" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="P59">
         <v>943693.99371889106</v>
@@ -6843,25 +6788,25 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D60" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E60" t="s">
         <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G60" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H60" t="s">
         <v>29</v>
       </c>
       <c r="I60" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="J60" t="s">
         <v>31</v>
@@ -6870,16 +6815,16 @@
         <v>32</v>
       </c>
       <c r="L60" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="M60">
         <v>0.99890621540189228</v>
       </c>
       <c r="N60" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="O60" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="P60">
         <v>1046631.847678181</v>
@@ -6935,25 +6880,25 @@
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D61" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E61" t="s">
         <v>37</v>
       </c>
       <c r="F61" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G61" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="H61" t="s">
         <v>38</v>
       </c>
       <c r="I61" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="J61" t="s">
         <v>40</v>
@@ -6962,16 +6907,16 @@
         <v>41</v>
       </c>
       <c r="L61" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="M61">
         <v>0.99988233990418507</v>
       </c>
       <c r="N61" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O61" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="P61">
         <v>10508.819966946419</v>
@@ -7021,6 +6966,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>